<commit_message>
readme format, screenshot update, title update
</commit_message>
<xml_diff>
--- a/FinOps tool evaluator - v1.01.xlsx
+++ b/FinOps tool evaluator - v1.01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ari08\Desktop\Git\finops-tool-evaluator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B51AB4-370D-4CCD-973A-F2D3C46891D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB6E763-E902-4597-B208-88868ED61590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="330">
   <si>
     <t>EC2</t>
   </si>
@@ -1055,6 +1055,9 @@
   </si>
   <si>
     <t>Cloud Financial Management (FinOps) tool evaluator - v1.01</t>
+  </si>
+  <si>
+    <t>Cloud Financial Management (FinOps) tool evaluator</t>
   </si>
 </sst>
 </file>
@@ -2038,9 +2041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41F69F1-798B-4E9F-89F8-0AAAC17B522F}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2347,9 +2348,9 @@
   </sheetPr>
   <dimension ref="A1:K396"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C402" sqref="C402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -2367,10 +2368,8 @@
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" collapsed="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="44" t="str">
-        <f>Cover!B2</f>
-        <v>Cloud Financial Management (FinOps) tool evaluator - v1.01</v>
+      <c r="B1" s="44" t="s">
+        <v>329</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>

</xml_diff>

<commit_message>
move comment to note column
</commit_message>
<xml_diff>
--- a/FinOps tool evaluator - v1.01.xlsx
+++ b/FinOps tool evaluator - v1.01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ari08\Desktop\Git\finops-tool-evaluator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB6E763-E902-4597-B208-88868ED61590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD31F8FA-21D7-4D74-8A13-3A79B759E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,44 +25,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Peter Shi</author>
-  </authors>
-  <commentList>
-    <comment ref="F69" authorId="0" shapeId="0" xr:uid="{EB5CF574-5797-4FE7-A3A0-4B2C53325761}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Unable to apply OR filter to multiple tags without use of AWS Cost Categories.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F124" authorId="0" shapeId="0" xr:uid="{659C4706-7C9C-4979-86E7-3F89B3ECA7F1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Requires data download and manipulation</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="332">
   <si>
     <t>EC2</t>
   </si>
@@ -1058,6 +1022,12 @@
   </si>
   <si>
     <t>Cloud Financial Management (FinOps) tool evaluator</t>
+  </si>
+  <si>
+    <t>Unable to apply OR filter to multiple tags without use of AWS Cost Categories.</t>
+  </si>
+  <si>
+    <t>Insight requires csv download and manipulation in excel</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1038,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1151,18 +1121,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1296,7 +1254,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1494,7 +1452,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="4" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -1503,6 +1461,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2341,16 +2305,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B857CC-25BE-4EEF-8055-F54D1741CE6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B857CC-25BE-4EEF-8055-F54D1741CE6E}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K396"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C402" sqref="C402"/>
+      <selection pane="bottomLeft" activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2324,8 @@
     <col min="3" max="3" width="52" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" style="54" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" customWidth="1"/>
@@ -3512,7 +3477,9 @@
       <c r="F69" s="36">
         <v>0.5</v>
       </c>
-      <c r="G69" s="36"/>
+      <c r="G69" s="75" t="s">
+        <v>330</v>
+      </c>
       <c r="H69" s="36"/>
       <c r="I69" s="63"/>
     </row>
@@ -4375,7 +4342,9 @@
       <c r="F124" s="33">
         <v>0.5</v>
       </c>
-      <c r="G124" s="33"/>
+      <c r="G124" s="76" t="s">
+        <v>331</v>
+      </c>
       <c r="H124" s="33"/>
       <c r="I124" s="61"/>
     </row>
@@ -8634,6 +8603,5 @@
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>